<commit_message>
Updated code changes of Employee, Manage ACL USers, Manager Login and Job Cards
</commit_message>
<xml_diff>
--- a/Auto-IT/Bulk-Jobs-Stable.xlsx
+++ b/Auto-IT/Bulk-Jobs-Stable.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2BCBD377-AAA0-449F-874D-378F0E260E8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{89BCCDEB-DB12-435F-A766-C569DE3D8D7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14600" windowHeight="1950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13960" windowHeight="5730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,13 @@
     <t>Security at DSO entrance</t>
   </si>
   <si>
-    <t>sativa</t>
-  </si>
-  <si>
-    <t>John Fred</t>
-  </si>
-  <si>
     <t>Security Duty-01</t>
+  </si>
+  <si>
+    <t>Zina</t>
+  </si>
+  <si>
+    <t>Sadio</t>
   </si>
 </sst>
 </file>
@@ -87,11 +87,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -314,7 +316,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -340,16 +342,16 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E2" s="2"/>
     </row>

</xml_diff>